<commit_message>
Added photos and readme
</commit_message>
<xml_diff>
--- a/Gripper/BOM/GripperBOM.xlsx
+++ b/Gripper/BOM/GripperBOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb3493921ac56168/Pulpit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BiggerProjects\Robotic-gripper\Gripper\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{31DB44B5-0A69-418D-945D-8EA94038EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3ED9DBA-3C13-43CE-93C6-CDFFBB82B268}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA1024E-39B7-4E38-8B8A-0C18293C05CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="50745" windowHeight="21840" xr2:uid="{B7010733-558F-45CB-B972-AB870968295A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -142,9 +142,6 @@
     <t>5x13x4mm</t>
   </si>
   <si>
-    <t>Servo horn</t>
-  </si>
-  <si>
     <t>Servo</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Application</t>
   </si>
   <si>
-    <t>TODO - fix names</t>
-  </si>
-  <si>
     <t>Top to mid(base)</t>
   </si>
   <si>
@@ -191,6 +185,9 @@
   </si>
   <si>
     <t>HZ03</t>
+  </si>
+  <si>
+    <t>Round aluminium servo horn</t>
   </si>
 </sst>
 </file>
@@ -266,13 +263,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,7 +589,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,17 +597,18 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -619,11 +617,11 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -648,11 +646,9 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -677,7 +673,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -703,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -723,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -783,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -803,7 +799,7 @@
         <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -823,7 +819,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -863,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -906,26 +902,26 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
@@ -934,10 +930,10 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="5"/>
       <c r="C21" t="s">
         <v>32</v>
       </c>
@@ -946,10 +942,10 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="5"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
@@ -958,37 +954,37 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="7"/>
+      <c r="A23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5"/>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
@@ -997,59 +993,59 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" t="s">
-        <v>37</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="7"/>
+      <c r="A29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="5"/>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
         <v>40</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" t="s">
-        <v>41</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="7"/>
+      <c r="A31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A18:E19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="A25:E26"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A18:E19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>

</xml_diff>

<commit_message>
Updating BOM +adding pcb spacers
</commit_message>
<xml_diff>
--- a/Gripper/BOM/GripperBOM.xlsx
+++ b/Gripper/BOM/GripperBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BiggerProjects\Robotic-gripper\Gripper\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA1024E-39B7-4E38-8B8A-0C18293C05CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9B80D2-D123-4DF9-8319-00B767B8BB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="50745" windowHeight="21840" xr2:uid="{B7010733-558F-45CB-B972-AB870968295A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Type</t>
   </si>
@@ -184,17 +184,47 @@
     <t>Mid to bottom(base), axles for sticks</t>
   </si>
   <si>
-    <t>HZ03</t>
-  </si>
-  <si>
     <t>Round aluminium servo horn</t>
+  </si>
+  <si>
+    <t>Wires</t>
+  </si>
+  <si>
+    <t>HZ03 Connector with pins</t>
+  </si>
+  <si>
+    <t>HZ02 Connector with pins</t>
+  </si>
+  <si>
+    <t>USB-C male plug(to solder wires)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Solder-Cable-Socket-Attached-Board/dp/B07P1BDNQV</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/15100</t>
+  </si>
+  <si>
+    <t>https://www.ebmia.pl/waleczki/37040-walek-waleczki-5x8-skf.html</t>
+  </si>
+  <si>
+    <t>https://botland.store/standard-servos/3576-servo-powerhd-lf-20mg-standard-6939670200387.html</t>
+  </si>
+  <si>
+    <t>https://en.maritex.com.pl/connectors/crimp_terminal_connectors/crimp_terminal_2_54mm_pitch/female_crimp_terminal_housings_for_cable_with_snap-lock_2_54_mm_pitch/hz03.html</t>
+  </si>
+  <si>
+    <t>https://en.maritex.com.pl/connectors/crimp_terminal_connectors/crimp_terminal_2_54mm_pitch/female_crimp_terminal_housings_for_cable_with_snap-lock_2_54_mm_pitch/hz02.html</t>
+  </si>
+  <si>
+    <t>Sample links</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +258,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -255,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -263,15 +302,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,15 +626,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7825B12-D591-4A48-A6A9-42A8F37A61E5}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
@@ -602,13 +642,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -617,11 +657,11 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -902,20 +942,23 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -930,22 +973,25 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="6"/>
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="6"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
@@ -954,31 +1000,31 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="5"/>
+      <c r="A23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="6"/>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -993,34 +1039,40 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="6"/>
       <c r="C28" t="s">
         <v>36</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="6"/>
       <c r="C29" t="s">
         <v>36</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="6"/>
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -1029,18 +1081,52 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="5"/>
+      <c r="A31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A18:E19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A27:B27"/>
+  <mergeCells count="16">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="A25:E26"/>
@@ -1049,6 +1135,11 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A18:E19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed BOM, added new pic
</commit_message>
<xml_diff>
--- a/Gripper/BOM/GripperBOM.xlsx
+++ b/Gripper/BOM/GripperBOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BiggerProjects\Robotic-gripper\Gripper\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CEFB44-264B-46B3-9DCB-9461D7521144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F0250-2213-4702-889D-4953A8F552FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="3720" windowWidth="37935" windowHeight="15885" xr2:uid="{B7010733-558F-45CB-B972-AB870968295A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Type</t>
   </si>
@@ -160,9 +160,6 @@
     <t>2,1/5,5mm</t>
   </si>
   <si>
-    <t>PCB to base, panel mount</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
@@ -239,6 +236,12 @@
   </si>
   <si>
     <t>optional</t>
+  </si>
+  <si>
+    <t>PCB to base, panel mount, usb-c mount</t>
+  </si>
+  <si>
+    <t>You may use angled goldpins connectors instead of WZ03/02 - then you don’t need HZ03/02 connectors</t>
   </si>
 </sst>
 </file>
@@ -363,9 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -378,20 +378,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +712,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,14 +725,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -738,39 +741,39 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="7" t="s">
-        <v>65</v>
+      <c r="K2" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>42</v>
+      <c r="F3" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="2"/>
@@ -780,23 +783,23 @@
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="11">
-        <v>4</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>41</v>
+      <c r="E4" s="10">
+        <v>6</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -806,226 +809,226 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>4</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" t="s">
+      <c r="O6" s="8"/>
+      <c r="P6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="10">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="10">
         <v>2</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="9"/>
-      <c r="P6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="F11" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="D12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="C13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10">
         <v>4</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="F14" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11">
-        <v>4</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="11">
-        <v>2</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="11">
-        <v>3</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11">
-        <v>4</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1035,22 +1038,22 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
       <c r="G19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1058,253 +1061,265 @@
         <v>4</v>
       </c>
       <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10">
+      <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
         <v>1</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="15"/>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>1</v>
       </c>
       <c r="G28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="9">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8">
         <v>1</v>
       </c>
-      <c r="G29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="9">
+      <c r="F32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="F33" t="s">
         <v>62</v>
       </c>
-      <c r="G31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="G33" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="F33" t="s">
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="F34" t="s">
         <v>63</v>
       </c>
-      <c r="G33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="F34" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="35" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
     </row>
     <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
+      <c r="H36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
     </row>
     <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
     </row>
     <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
     </row>
     <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A25:E26"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A18:E19"/>
     <mergeCell ref="A22:B22"/>
@@ -1312,15 +1327,6 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="A25:E26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>